<commit_message>
Added create new table
- In gui you can create your own schedule
</commit_message>
<xml_diff>
--- a/automate/תבנית זמינות.xlsx
+++ b/automate/תבנית זמינות.xlsx
@@ -985,37 +985,13 @@
       <c r="R1" s="5" t="n"/>
     </row>
     <row r="2" ht="18" customHeight="1">
-      <c r="A2" s="17" t="inlineStr">
-        <is>
-          <t>יניב שטיינר</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>b.c</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
+      <c r="A2" s="17" t="n"/>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="2" t="n"/>
       <c r="D2" s="1" t="n"/>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>a.b</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
+      <c r="E2" s="1" t="n"/>
+      <c r="F2" s="1" t="n"/>
+      <c r="G2" s="1" t="n"/>
       <c r="H2" s="1" t="n"/>
       <c r="I2" s="18" t="n">
         <v>6</v>
@@ -1031,11 +1007,7 @@
         </is>
       </c>
       <c r="N2" s="5" t="n"/>
-      <c r="O2" s="45" t="inlineStr">
-        <is>
-          <t>תקופת מבחנים ובשבת נמצא בשבת חתן</t>
-        </is>
-      </c>
+      <c r="O2" s="45" t="n"/>
       <c r="P2" s="5" t="n"/>
       <c r="Q2" s="37" t="n">
         <v>1</v>
@@ -1043,34 +1015,14 @@
       <c r="R2" s="5" t="n"/>
     </row>
     <row r="3" ht="21.4" customHeight="1">
-      <c r="A3" s="19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">אוראל </t>
-        </is>
-      </c>
+      <c r="A3" s="19" t="n"/>
       <c r="B3" s="2" t="n"/>
       <c r="C3" s="2" t="n"/>
       <c r="D3" s="1" t="n"/>
-      <c r="E3" s="1" t="inlineStr">
-        <is>
-          <t>b.c</t>
-        </is>
-      </c>
-      <c r="F3" s="1" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="G3" s="1" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="H3" s="1" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
+      <c r="E3" s="1" t="n"/>
+      <c r="F3" s="1" t="n"/>
+      <c r="G3" s="1" t="n"/>
+      <c r="H3" s="1" t="n"/>
       <c r="I3" s="20" t="n">
         <v>6</v>
       </c>
@@ -1093,46 +1045,14 @@
       <c r="R3" s="5" t="n"/>
     </row>
     <row r="4" ht="20.65" customHeight="1">
-      <c r="A4" s="21" t="inlineStr">
-        <is>
-          <t>אמור טלבי</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>b.c</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
+      <c r="A4" s="21" t="n"/>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="2" t="n"/>
+      <c r="E4" s="1" t="n"/>
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="1" t="n"/>
       <c r="I4" s="22" t="n">
         <v>6</v>
       </c>
@@ -1147,11 +1067,7 @@
         </is>
       </c>
       <c r="N4" s="5" t="n"/>
-      <c r="O4" s="45" t="inlineStr">
-        <is>
-          <t>מי שלא מוחא כפיים..</t>
-        </is>
-      </c>
+      <c r="O4" s="45" t="n"/>
       <c r="P4" s="5" t="n"/>
       <c r="Q4" s="39" t="n">
         <v>1</v>
@@ -1159,28 +1075,12 @@
       <c r="R4" s="5" t="n"/>
     </row>
     <row r="5" ht="19.15" customHeight="1">
-      <c r="A5" s="23" t="inlineStr">
-        <is>
-          <t>עמית בלסן</t>
-        </is>
-      </c>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
+      <c r="A5" s="23" t="n"/>
+      <c r="B5" s="1" t="n"/>
       <c r="C5" s="1" t="n"/>
-      <c r="D5" s="1" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
+      <c r="D5" s="1" t="n"/>
       <c r="E5" s="1" t="n"/>
-      <c r="F5" s="1" t="inlineStr">
-        <is>
-          <t>b.c</t>
-        </is>
-      </c>
+      <c r="F5" s="1" t="n"/>
       <c r="G5" s="1" t="n"/>
       <c r="H5" s="1" t="n"/>
       <c r="I5" s="24" t="n">
@@ -1205,46 +1105,14 @@
       <c r="R5" s="5" t="n"/>
     </row>
     <row r="6" ht="18" customHeight="1">
-      <c r="A6" s="25" t="inlineStr">
-        <is>
-          <t>אור</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="E6" s="1" t="inlineStr">
-        <is>
-          <t>a.c</t>
-        </is>
-      </c>
-      <c r="F6" s="1" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="G6" s="1" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="H6" s="1" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
+      <c r="A6" s="25" t="n"/>
+      <c r="B6" s="1" t="n"/>
+      <c r="C6" s="1" t="n"/>
+      <c r="D6" s="1" t="n"/>
+      <c r="E6" s="1" t="n"/>
+      <c r="F6" s="1" t="n"/>
+      <c r="G6" s="1" t="n"/>
+      <c r="H6" s="1" t="n"/>
       <c r="I6" s="26" t="n">
         <v>6</v>
       </c>
@@ -1267,42 +1135,14 @@
       <c r="R6" s="5" t="n"/>
     </row>
     <row r="7" ht="19.9" customHeight="1">
-      <c r="A7" s="27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">זיו שהינו </t>
-        </is>
-      </c>
-      <c r="B7" s="1" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
+      <c r="A7" s="27" t="n"/>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="2" t="n"/>
       <c r="D7" s="1" t="n"/>
-      <c r="E7" s="1" t="inlineStr">
-        <is>
-          <t>b.c</t>
-        </is>
-      </c>
-      <c r="F7" s="1" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="G7" s="1" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="H7" s="1" t="inlineStr">
-        <is>
-          <t>a.b</t>
-        </is>
-      </c>
+      <c r="E7" s="1" t="n"/>
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" s="1" t="n"/>
+      <c r="H7" s="1" t="n"/>
       <c r="I7" s="28" t="n">
         <v>6</v>
       </c>
@@ -1325,42 +1165,14 @@
       <c r="R7" s="5" t="n"/>
     </row>
     <row r="8" ht="18.4" customHeight="1" thickBot="1">
-      <c r="A8" s="29" t="inlineStr">
-        <is>
-          <t>רוני</t>
-        </is>
-      </c>
+      <c r="A8" s="29" t="n"/>
       <c r="B8" s="13" t="n"/>
-      <c r="C8" s="12" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="D8" s="12" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="E8" s="13" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="F8" s="13" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="G8" s="13" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="H8" s="13" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
+      <c r="C8" s="12" t="n"/>
+      <c r="D8" s="12" t="n"/>
+      <c r="E8" s="13" t="n"/>
+      <c r="F8" s="13" t="n"/>
+      <c r="G8" s="13" t="n"/>
+      <c r="H8" s="13" t="n"/>
       <c r="I8" s="30" t="n">
         <v>6</v>
       </c>

</xml_diff>